<commit_message>
Git Path Set for release notes
Git Path Set for release notes in ECO file for release note documents
</commit_message>
<xml_diff>
--- a/SR Smart App/ECO_SRSMART_ANDROID_01.01.10.xlsx
+++ b/SR Smart App/ECO_SRSMART_ANDROID_01.01.10.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="20" windowWidth="25600" windowHeight="14160"/>
+    <workbookView xWindow="1580" yWindow="0" windowWidth="25600" windowHeight="14160"/>
   </bookViews>
   <sheets>
     <sheet name="ECO FORM" sheetId="1" r:id="rId1"/>
@@ -147,20 +147,20 @@
     <t>ECO Form V1.2</t>
   </si>
   <si>
-    <t xml:space="preserve">Git Hub Path - &gt; relase note
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>SecuRemote Smart Mobile Application</t>
+  </si>
+  <si>
+    <t>SR Smart Mobile App will operate various SR products like Smart Deadbolt, Keeler,GDO,SR DevKit.</t>
+  </si>
+  <si>
+    <t>App Version - 01.01.10 , Build Version - 01.01.38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RELEASENOTE_SRSMART_ANDROID_01.01.10.docx  - https://github.com/DelphianSystems/SecuRemote/tree/master/SR%20Smart%20App
 </t>
-  </si>
-  <si>
-    <t>Customer</t>
-  </si>
-  <si>
-    <t>SecuRemote Smart Mobile Application</t>
-  </si>
-  <si>
-    <t>SR Smart Mobile App will operate various SR products like Smart Deadbolt, Keeler,GDO,SR DevKit.</t>
-  </si>
-  <si>
-    <t>App Version - 01.01.10 , Build Version - 01.01.38</t>
   </si>
 </sst>
 </file>
@@ -189,14 +189,6 @@
       <b/>
       <sz val="8"/>
       <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color indexed="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
@@ -265,6 +257,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="8"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="6">
@@ -477,44 +474,47 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -566,34 +566,34 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -632,12 +632,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="5"/>
     </xf>
@@ -648,11 +648,74 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -674,80 +737,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="14">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -760,6 +760,7 @@
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -962,8 +963,8 @@
         <xdr:to>
           <xdr:col>3</xdr:col>
           <xdr:colOff>101600</xdr:colOff>
-          <xdr:row>11</xdr:row>
-          <xdr:rowOff>177800</xdr:rowOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>1953</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1023,8 +1024,8 @@
         <xdr:to>
           <xdr:col>4</xdr:col>
           <xdr:colOff>101600</xdr:colOff>
-          <xdr:row>11</xdr:row>
-          <xdr:rowOff>177800</xdr:rowOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>1953</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1084,8 +1085,8 @@
         <xdr:to>
           <xdr:col>5</xdr:col>
           <xdr:colOff>165100</xdr:colOff>
-          <xdr:row>11</xdr:row>
-          <xdr:rowOff>177800</xdr:rowOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>1953</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1145,8 +1146,8 @@
         <xdr:to>
           <xdr:col>6</xdr:col>
           <xdr:colOff>38100</xdr:colOff>
-          <xdr:row>11</xdr:row>
-          <xdr:rowOff>177800</xdr:rowOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>1953</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1206,8 +1207,8 @@
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>787400</xdr:colOff>
-          <xdr:row>18</xdr:row>
-          <xdr:rowOff>177800</xdr:rowOff>
+          <xdr:row>19</xdr:row>
+          <xdr:rowOff>1954</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1267,8 +1268,8 @@
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>787400</xdr:colOff>
-          <xdr:row>18</xdr:row>
-          <xdr:rowOff>177800</xdr:rowOff>
+          <xdr:row>19</xdr:row>
+          <xdr:rowOff>1954</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1328,8 +1329,8 @@
         <xdr:to>
           <xdr:col>5</xdr:col>
           <xdr:colOff>317500</xdr:colOff>
-          <xdr:row>18</xdr:row>
-          <xdr:rowOff>177800</xdr:rowOff>
+          <xdr:row>19</xdr:row>
+          <xdr:rowOff>1954</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1450,8 +1451,8 @@
         <xdr:to>
           <xdr:col>6</xdr:col>
           <xdr:colOff>482600</xdr:colOff>
-          <xdr:row>18</xdr:row>
-          <xdr:rowOff>177800</xdr:rowOff>
+          <xdr:row>19</xdr:row>
+          <xdr:rowOff>1954</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1999,8 +2000,8 @@
         <xdr:to>
           <xdr:col>5</xdr:col>
           <xdr:colOff>38100</xdr:colOff>
-          <xdr:row>10</xdr:row>
-          <xdr:rowOff>177800</xdr:rowOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>1954</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2243,8 +2244,8 @@
         <xdr:to>
           <xdr:col>7</xdr:col>
           <xdr:colOff>952500</xdr:colOff>
-          <xdr:row>11</xdr:row>
-          <xdr:rowOff>177800</xdr:rowOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>1953</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2932,7 +2933,7 @@
   <dimension ref="A1:H73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2981,135 +2982,135 @@
       <c r="D3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="44" t="s">
+      <c r="E3" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="45"/>
+      <c r="F3" s="62"/>
       <c r="G3" s="10" t="s">
         <v>4</v>
       </c>
       <c r="H3" s="43" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="15" customHeight="1">
       <c r="B4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="46" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="48"/>
+      <c r="C4" s="67" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="68"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="68"/>
+      <c r="G4" s="68"/>
+      <c r="H4" s="69"/>
     </row>
     <row r="5" spans="2:8" ht="28" customHeight="1">
       <c r="B5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="46" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="48"/>
+      <c r="C5" s="67" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="69"/>
     </row>
     <row r="6" spans="2:8">
-      <c r="B6" s="49"/>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="50"/>
-      <c r="H6" s="51"/>
+      <c r="B6" s="70"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="71"/>
+      <c r="H6" s="72"/>
     </row>
     <row r="7" spans="2:8">
       <c r="B7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="52"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
-      <c r="F7" s="52"/>
-      <c r="G7" s="52"/>
-      <c r="H7" s="52"/>
+      <c r="C7" s="73"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="73"/>
+      <c r="F7" s="73"/>
+      <c r="G7" s="73"/>
+      <c r="H7" s="73"/>
     </row>
     <row r="8" spans="2:8">
-      <c r="B8" s="53"/>
-      <c r="C8" s="53"/>
-      <c r="D8" s="53"/>
-      <c r="E8" s="53"/>
-      <c r="F8" s="53"/>
-      <c r="G8" s="53"/>
-      <c r="H8" s="53"/>
+      <c r="B8" s="63"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="63"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="63"/>
+      <c r="G8" s="63"/>
+      <c r="H8" s="63"/>
     </row>
     <row r="9" spans="2:8" ht="38" customHeight="1">
       <c r="B9" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="54" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="55"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="55"/>
-      <c r="G9" s="55"/>
-      <c r="H9" s="56"/>
+      <c r="C9" s="74" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="75"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="75"/>
+      <c r="G9" s="75"/>
+      <c r="H9" s="76"/>
     </row>
     <row r="10" spans="2:8">
-      <c r="B10" s="57" t="s">
+      <c r="B10" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="58"/>
-      <c r="D10" s="58"/>
-      <c r="E10" s="58"/>
-      <c r="F10" s="58"/>
-      <c r="G10" s="58"/>
-      <c r="H10" s="59"/>
+      <c r="C10" s="65"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="65"/>
+      <c r="H10" s="66"/>
     </row>
     <row r="11" spans="2:8">
-      <c r="B11" s="60" t="s">
+      <c r="B11" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="60"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="60"/>
-      <c r="H11" s="60"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="58"/>
+      <c r="E11" s="58"/>
+      <c r="F11" s="58"/>
+      <c r="G11" s="58"/>
+      <c r="H11" s="58"/>
     </row>
     <row r="12" spans="2:8">
       <c r="B12" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="60"/>
-      <c r="D12" s="60"/>
-      <c r="E12" s="60"/>
-      <c r="F12" s="60"/>
-      <c r="G12" s="60"/>
-      <c r="H12" s="60"/>
+      <c r="C12" s="58"/>
+      <c r="D12" s="58"/>
+      <c r="E12" s="58"/>
+      <c r="F12" s="58"/>
+      <c r="G12" s="58"/>
+      <c r="H12" s="58"/>
     </row>
     <row r="13" spans="2:8">
-      <c r="B13" s="60"/>
-      <c r="C13" s="60"/>
-      <c r="D13" s="60"/>
-      <c r="E13" s="60"/>
-      <c r="F13" s="60"/>
-      <c r="G13" s="60"/>
-      <c r="H13" s="60"/>
+      <c r="B13" s="58"/>
+      <c r="C13" s="58"/>
+      <c r="D13" s="58"/>
+      <c r="E13" s="58"/>
+      <c r="F13" s="58"/>
+      <c r="G13" s="58"/>
+      <c r="H13" s="58"/>
     </row>
     <row r="14" spans="2:8">
-      <c r="B14" s="44"/>
+      <c r="B14" s="60"/>
       <c r="C14" s="61"/>
       <c r="D14" s="61"/>
       <c r="E14" s="61"/>
       <c r="F14" s="61"/>
       <c r="G14" s="61"/>
-      <c r="H14" s="45"/>
+      <c r="H14" s="62"/>
     </row>
     <row r="15" spans="2:8">
       <c r="B15" s="9" t="s">
@@ -3131,112 +3132,112 @@
       <c r="H15" s="5"/>
     </row>
     <row r="16" spans="2:8">
-      <c r="B16" s="60"/>
-      <c r="C16" s="60"/>
-      <c r="D16" s="60"/>
-      <c r="E16" s="60"/>
-      <c r="F16" s="60"/>
-      <c r="G16" s="60"/>
-      <c r="H16" s="60"/>
+      <c r="B16" s="58"/>
+      <c r="C16" s="58"/>
+      <c r="D16" s="58"/>
+      <c r="E16" s="58"/>
+      <c r="F16" s="58"/>
+      <c r="G16" s="58"/>
+      <c r="H16" s="58"/>
     </row>
     <row r="17" spans="2:8">
       <c r="B17" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="60" t="s">
+      <c r="C17" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="60"/>
-      <c r="E17" s="60" t="s">
+      <c r="D17" s="58"/>
+      <c r="E17" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="F17" s="60"/>
-      <c r="G17" s="60"/>
-      <c r="H17" s="60"/>
+      <c r="F17" s="58"/>
+      <c r="G17" s="58"/>
+      <c r="H17" s="58"/>
     </row>
     <row r="18" spans="2:8">
       <c r="B18" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="60" t="s">
+      <c r="C18" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="60"/>
+      <c r="D18" s="58"/>
       <c r="E18" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F18" s="62"/>
-      <c r="G18" s="62"/>
+      <c r="F18" s="59"/>
+      <c r="G18" s="59"/>
       <c r="H18" s="5"/>
     </row>
     <row r="19" spans="2:8">
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
-      <c r="D19" s="60"/>
-      <c r="E19" s="60"/>
-      <c r="F19" s="60"/>
-      <c r="G19" s="60"/>
-      <c r="H19" s="60"/>
+      <c r="D19" s="58"/>
+      <c r="E19" s="58"/>
+      <c r="F19" s="58"/>
+      <c r="G19" s="58"/>
+      <c r="H19" s="58"/>
     </row>
     <row r="20" spans="2:8">
-      <c r="B20" s="60"/>
-      <c r="C20" s="60"/>
-      <c r="D20" s="60"/>
-      <c r="E20" s="60"/>
-      <c r="F20" s="60"/>
-      <c r="G20" s="60"/>
-      <c r="H20" s="60"/>
+      <c r="B20" s="58"/>
+      <c r="C20" s="58"/>
+      <c r="D20" s="58"/>
+      <c r="E20" s="58"/>
+      <c r="F20" s="58"/>
+      <c r="G20" s="58"/>
+      <c r="H20" s="58"/>
     </row>
     <row r="21" spans="2:8">
       <c r="B21" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C21" s="5"/>
-      <c r="D21" s="60" t="s">
+      <c r="D21" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="E21" s="60"/>
-      <c r="F21" s="60"/>
-      <c r="G21" s="60"/>
-      <c r="H21" s="60"/>
+      <c r="E21" s="58"/>
+      <c r="F21" s="58"/>
+      <c r="G21" s="58"/>
+      <c r="H21" s="58"/>
     </row>
     <row r="22" spans="2:8" ht="15" customHeight="1">
-      <c r="B22" s="68" t="s">
+      <c r="B22" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="69"/>
-      <c r="D22" s="69"/>
-      <c r="E22" s="69"/>
-      <c r="F22" s="69"/>
-      <c r="G22" s="69"/>
-      <c r="H22" s="70"/>
+      <c r="C22" s="50"/>
+      <c r="D22" s="50"/>
+      <c r="E22" s="50"/>
+      <c r="F22" s="50"/>
+      <c r="G22" s="50"/>
+      <c r="H22" s="51"/>
     </row>
     <row r="23" spans="2:8">
-      <c r="B23" s="71"/>
-      <c r="C23" s="72"/>
-      <c r="D23" s="72"/>
-      <c r="E23" s="72"/>
-      <c r="F23" s="72"/>
-      <c r="G23" s="72"/>
-      <c r="H23" s="73"/>
+      <c r="B23" s="52"/>
+      <c r="C23" s="53"/>
+      <c r="D23" s="53"/>
+      <c r="E23" s="53"/>
+      <c r="F23" s="53"/>
+      <c r="G23" s="53"/>
+      <c r="H23" s="54"/>
     </row>
     <row r="24" spans="2:8">
-      <c r="B24" s="71"/>
-      <c r="C24" s="72"/>
-      <c r="D24" s="72"/>
-      <c r="E24" s="72"/>
-      <c r="F24" s="72"/>
-      <c r="G24" s="72"/>
-      <c r="H24" s="73"/>
+      <c r="B24" s="52"/>
+      <c r="C24" s="53"/>
+      <c r="D24" s="53"/>
+      <c r="E24" s="53"/>
+      <c r="F24" s="53"/>
+      <c r="G24" s="53"/>
+      <c r="H24" s="54"/>
     </row>
     <row r="25" spans="2:8">
-      <c r="B25" s="74"/>
-      <c r="C25" s="75"/>
-      <c r="D25" s="75"/>
-      <c r="E25" s="75"/>
-      <c r="F25" s="75"/>
-      <c r="G25" s="75"/>
-      <c r="H25" s="76"/>
+      <c r="B25" s="55"/>
+      <c r="C25" s="56"/>
+      <c r="D25" s="56"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="56"/>
+      <c r="G25" s="56"/>
+      <c r="H25" s="57"/>
     </row>
     <row r="26" spans="2:8">
       <c r="B26" s="9" t="s">
@@ -3302,11 +3303,11 @@
       <c r="C31" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D31" s="63" t="s">
+      <c r="D31" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="E31" s="64"/>
-      <c r="F31" s="65"/>
+      <c r="E31" s="45"/>
+      <c r="F31" s="46"/>
       <c r="G31" s="5" t="s">
         <v>1</v>
       </c>
@@ -3317,11 +3318,11 @@
       <c r="C32" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D32" s="63" t="s">
+      <c r="D32" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="E32" s="64"/>
-      <c r="F32" s="65"/>
+      <c r="E32" s="45"/>
+      <c r="F32" s="46"/>
       <c r="G32" s="20" t="s">
         <v>1</v>
       </c>
@@ -3332,11 +3333,11 @@
         <v>30</v>
       </c>
       <c r="C33" s="23"/>
-      <c r="D33" s="63" t="s">
+      <c r="D33" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="E33" s="64"/>
-      <c r="F33" s="65"/>
+      <c r="E33" s="45"/>
+      <c r="F33" s="46"/>
       <c r="G33" s="5" t="s">
         <v>1</v>
       </c>
@@ -3358,12 +3359,12 @@
       <c r="C35" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="D35" s="66" t="s">
+      <c r="D35" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="E35" s="67"/>
+      <c r="E35" s="48"/>
       <c r="F35" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G35" s="27" t="s">
         <v>33</v>
@@ -3507,44 +3508,52 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="B22:H25"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="B8:H8"/>
+    <mergeCell ref="C9:H9"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="C12:H12"/>
+    <mergeCell ref="B13:H13"/>
+    <mergeCell ref="B14:H14"/>
+    <mergeCell ref="B16:H16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:H17"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="F18:G18"/>
     <mergeCell ref="D19:H19"/>
     <mergeCell ref="B20:H20"/>
     <mergeCell ref="D21:E21"/>
     <mergeCell ref="F21:H21"/>
-    <mergeCell ref="B13:H13"/>
-    <mergeCell ref="B14:H14"/>
-    <mergeCell ref="B16:H16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:H17"/>
-    <mergeCell ref="B8:H8"/>
-    <mergeCell ref="C9:H9"/>
-    <mergeCell ref="B10:H10"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="C12:H12"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="B6:H6"/>
-    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="B22:H25"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C9" r:id="rId1"/>
+    <hyperlink ref="D9" r:id="rId2" display="https://github.com/DelphianSystems/SecuRemote/tree/master/SR Smart App"/>
+    <hyperlink ref="E9" r:id="rId3" display="https://github.com/DelphianSystems/SecuRemote/tree/master/SR Smart App"/>
+    <hyperlink ref="F9" r:id="rId4" display="https://github.com/DelphianSystems/SecuRemote/tree/master/SR Smart App"/>
+    <hyperlink ref="G9" r:id="rId5" display="https://github.com/DelphianSystems/SecuRemote/tree/master/SR Smart App"/>
+    <hyperlink ref="H9" r:id="rId6" display="https://github.com/DelphianSystems/SecuRemote/tree/master/SR Smart App"/>
+  </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <drawing r:id="rId7"/>
+  <legacyDrawing r:id="rId8"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x14">
       <controls>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2049" r:id="rId3" name="Check Box 1">
+            <control shapeId="2049" r:id="rId9" name="Check Box 1">
               <controlPr defaultSize="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3567,7 +3576,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2050" r:id="rId4" name="Check Box 2">
+            <control shapeId="2050" r:id="rId10" name="Check Box 2">
               <controlPr defaultSize="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3579,8 +3588,8 @@
                   <to>
                     <xdr:col>3</xdr:col>
                     <xdr:colOff>101600</xdr:colOff>
-                    <xdr:row>11</xdr:row>
-                    <xdr:rowOff>177800</xdr:rowOff>
+                    <xdr:row>12</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3590,7 +3599,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2051" r:id="rId5" name="Check Box 3">
+            <control shapeId="2051" r:id="rId11" name="Check Box 3">
               <controlPr defaultSize="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3602,8 +3611,8 @@
                   <to>
                     <xdr:col>4</xdr:col>
                     <xdr:colOff>101600</xdr:colOff>
-                    <xdr:row>11</xdr:row>
-                    <xdr:rowOff>177800</xdr:rowOff>
+                    <xdr:row>12</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3613,7 +3622,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2052" r:id="rId6" name="Check Box 4">
+            <control shapeId="2052" r:id="rId12" name="Check Box 4">
               <controlPr defaultSize="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3625,8 +3634,8 @@
                   <to>
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>165100</xdr:colOff>
-                    <xdr:row>11</xdr:row>
-                    <xdr:rowOff>177800</xdr:rowOff>
+                    <xdr:row>12</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3636,7 +3645,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2053" r:id="rId7" name="Check Box 5">
+            <control shapeId="2053" r:id="rId13" name="Check Box 5">
               <controlPr defaultSize="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3648,8 +3657,8 @@
                   <to>
                     <xdr:col>6</xdr:col>
                     <xdr:colOff>38100</xdr:colOff>
-                    <xdr:row>11</xdr:row>
-                    <xdr:rowOff>177800</xdr:rowOff>
+                    <xdr:row>12</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3659,7 +3668,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2054" r:id="rId8" name="Check Box 6">
+            <control shapeId="2054" r:id="rId14" name="Check Box 6">
               <controlPr defaultSize="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3671,8 +3680,8 @@
                   <to>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>787400</xdr:colOff>
-                    <xdr:row>18</xdr:row>
-                    <xdr:rowOff>177800</xdr:rowOff>
+                    <xdr:row>19</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3682,7 +3691,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2055" r:id="rId9" name="Check Box 7">
+            <control shapeId="2055" r:id="rId15" name="Check Box 7">
               <controlPr defaultSize="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3694,8 +3703,8 @@
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>787400</xdr:colOff>
-                    <xdr:row>18</xdr:row>
-                    <xdr:rowOff>177800</xdr:rowOff>
+                    <xdr:row>19</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3705,7 +3714,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2056" r:id="rId10" name="Check Box 8">
+            <control shapeId="2056" r:id="rId16" name="Check Box 8">
               <controlPr defaultSize="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3717,8 +3726,8 @@
                   <to>
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>317500</xdr:colOff>
-                    <xdr:row>18</xdr:row>
-                    <xdr:rowOff>177800</xdr:rowOff>
+                    <xdr:row>19</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3728,7 +3737,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2057" r:id="rId11" name="Check Box 9">
+            <control shapeId="2057" r:id="rId17" name="Check Box 9">
               <controlPr defaultSize="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3751,7 +3760,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2058" r:id="rId12" name="Check Box 10">
+            <control shapeId="2058" r:id="rId18" name="Check Box 10">
               <controlPr defaultSize="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3763,8 +3772,8 @@
                   <to>
                     <xdr:col>6</xdr:col>
                     <xdr:colOff>482600</xdr:colOff>
-                    <xdr:row>18</xdr:row>
-                    <xdr:rowOff>177800</xdr:rowOff>
+                    <xdr:row>19</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3774,7 +3783,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2060" r:id="rId13" name="Check Box 12">
+            <control shapeId="2060" r:id="rId19" name="Check Box 12">
               <controlPr defaultSize="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3797,7 +3806,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2061" r:id="rId14" name="Check Box 13">
+            <control shapeId="2061" r:id="rId20" name="Check Box 13">
               <controlPr defaultSize="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3820,7 +3829,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2063" r:id="rId15" name="Check Box 15">
+            <control shapeId="2063" r:id="rId21" name="Check Box 15">
               <controlPr defaultSize="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3843,7 +3852,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2069" r:id="rId16" name="Check Box 21">
+            <control shapeId="2069" r:id="rId22" name="Check Box 21">
               <controlPr defaultSize="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3866,7 +3875,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2070" r:id="rId17" name="Check Box 22">
+            <control shapeId="2070" r:id="rId23" name="Check Box 22">
               <controlPr defaultSize="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3889,7 +3898,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2071" r:id="rId18" name="Check Box 23">
+            <control shapeId="2071" r:id="rId24" name="Check Box 23">
               <controlPr defaultSize="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3912,7 +3921,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2072" r:id="rId19" name="Check Box 24">
+            <control shapeId="2072" r:id="rId25" name="Check Box 24">
               <controlPr defaultSize="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3935,7 +3944,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2073" r:id="rId20" name="Check Box 25">
+            <control shapeId="2073" r:id="rId26" name="Check Box 25">
               <controlPr defaultSize="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3947,8 +3956,8 @@
                   <to>
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>38100</xdr:colOff>
-                    <xdr:row>10</xdr:row>
-                    <xdr:rowOff>177800</xdr:rowOff>
+                    <xdr:row>11</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3958,7 +3967,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2074" r:id="rId21" name="Check Box 26">
+            <control shapeId="2074" r:id="rId27" name="Check Box 26">
               <controlPr defaultSize="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3981,7 +3990,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2075" r:id="rId22" name="Check Box 27">
+            <control shapeId="2075" r:id="rId28" name="Check Box 27">
               <controlPr defaultSize="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4004,7 +4013,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2076" r:id="rId23" name="Check Box 28">
+            <control shapeId="2076" r:id="rId29" name="Check Box 28">
               <controlPr defaultSize="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4027,20 +4036,20 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2077" r:id="rId24" name="Check Box 29">
+            <control shapeId="2077" r:id="rId30" name="Check Box 29">
               <controlPr defaultSize="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>6</xdr:col>
                     <xdr:colOff>139700</xdr:colOff>
-                    <xdr:row>10</xdr:row>
-                    <xdr:rowOff>177800</xdr:rowOff>
+                    <xdr:row>11</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>7</xdr:col>
                     <xdr:colOff>952500</xdr:colOff>
-                    <xdr:row>11</xdr:row>
-                    <xdr:rowOff>177800</xdr:rowOff>
+                    <xdr:row>12</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4050,7 +4059,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2065" r:id="rId25" name="Check Box 17">
+            <control shapeId="2065" r:id="rId31" name="Check Box 17">
               <controlPr defaultSize="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4073,7 +4082,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2080" r:id="rId26" name="Check Box 32">
+            <control shapeId="2080" r:id="rId32" name="Check Box 17">
               <controlPr defaultSize="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4096,7 +4105,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2084" r:id="rId27" name="Check Box 36">
+            <control shapeId="2084" r:id="rId33" name="Check Box 28">
               <controlPr defaultSize="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4119,7 +4128,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2086" r:id="rId28" name="Check Box 38">
+            <control shapeId="2086" r:id="rId34" name="Check Box 38">
               <controlPr defaultSize="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4142,7 +4151,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2087" r:id="rId29" name="Check Box 39">
+            <control shapeId="2087" r:id="rId35" name="Check Box 39">
               <controlPr defaultSize="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4165,7 +4174,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="2089" r:id="rId30" name="Check Box 41">
+            <control shapeId="2089" r:id="rId36" name="Check Box 41">
               <controlPr defaultSize="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>

</xml_diff>